<commit_message>
new questions document and changed excel
</commit_message>
<xml_diff>
--- a/ProjectFiles/HotelIndeling.xlsx
+++ b/ProjectFiles/HotelIndeling.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\P_jaz\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\P_jaz\source\repos\HoteAtThelLock\ProjectFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{39B9FF74-9611-4506-87EC-9DC73DBF26B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766BB447-84BB-4F52-AE6E-B21E1D9C5F31}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{A5C215F7-F264-44C2-A50C-95F5043C020A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="14">
   <si>
     <t>kamer</t>
   </si>
@@ -64,13 +64,16 @@
   </si>
   <si>
     <t>Receptie</t>
+  </si>
+  <si>
+    <t>empty</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,8 +110,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -154,6 +164,11 @@
         <bgColor theme="7" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="6">
     <border>
@@ -231,7 +246,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -239,11 +254,11 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
@@ -253,6 +268,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -262,14 +278,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="7"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="20% - Accent1" xfId="4" builtinId="30"/>
     <cellStyle name="40% - Accent1" xfId="5" builtinId="31"/>
     <cellStyle name="60% - Accent1" xfId="6" builtinId="32"/>
     <cellStyle name="Controlecel" xfId="3" builtinId="23"/>
     <cellStyle name="Goed" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutraal" xfId="7" builtinId="28"/>
     <cellStyle name="Ongeldig" xfId="2" builtinId="27"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -583,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92E86E3D-C7D0-4F5C-A8C0-D00EC3D19987}">
-  <dimension ref="B3:I19"/>
+  <dimension ref="B2:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,261 +619,266 @@
     <col min="11" max="11" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="B10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G10" s="4" t="s">
+      <c r="E10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="H10" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H11" s="8" t="s">
+      <c r="B11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="15"/>
+      <c r="E11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="I11" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="B12" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="I12" s="9" t="s">
+      <c r="E12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E13" s="4" t="s">
+      <c r="B13" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="I13" s="9" t="s">
+      <c r="H13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I13" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14" s="4" t="s">
+      <c r="B14" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="I14" s="9" t="s">
+      <c r="H14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D15" s="4" t="s">
+      <c r="B15" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="I15" s="9" t="s">
+      <c r="G15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I15" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" s="4" t="s">
+      <c r="B16" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="I16" s="9" t="s">
+      <c r="G16" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I16" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="17" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D17" s="8" t="s">
+      <c r="B17" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G17" s="4" t="s">
+      <c r="E17" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H17" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I17" s="9" t="s">
+      <c r="I17" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D18" s="8" t="s">
+      <c r="B18" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="G18" s="4" t="s">
+      <c r="E18" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I18" s="9" t="s">
+      <c r="I18" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C19" s="12" t="s">
@@ -866,7 +889,7 @@
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
       <c r="H19" s="14"/>
-      <c r="I19" s="9" t="s">
+      <c r="I19" s="8" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>